<commit_message>
Refactor field options and enhance Excel handling by adding a helper function to extract plain text from Excel cells. Remove outdated blueprint_services.xlsx file and update blueprint_task_products.xlsx for improved data consistency and handling.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_task_products.xlsx
+++ b/input_tables/blueprint_task_products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve">taskProduct</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">roomplan FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preconInput</t>
   </si>
   <si>
     <t xml:space="preserve">Panos</t>
@@ -211,7 +214,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,16 +257,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -291,15 +295,16 @@
       <c r="A15" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>15</v>
       </c>
-    </row>
+      <c r="B16" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>16</v>
@@ -314,16 +319,13 @@
       <c r="A20" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,15 +333,24 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>8</v>
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update field_options.json for consistent task naming conventions and add new blueprint Excel files for improved data organization. Rename tasks to use hyphens and introduce new task categories for better clarity.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_task_products.xlsx
+++ b/input_tables/blueprint_task_products.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">dslr_captures</t>
   </si>
   <si>
-    <t xml:space="preserve">roomplan FP</t>
+    <t xml:space="preserve">roomplan-FP</t>
   </si>
   <si>
     <t xml:space="preserve">preconInput</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Flythrough</t>
   </si>
   <si>
-    <t xml:space="preserve">Walkthrough video</t>
+    <t xml:space="preserve">Walkthrough-video</t>
   </si>
   <si>
     <t xml:space="preserve">Hdr-images</t>
@@ -213,8 +213,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>